<commit_message>
Restructure the project, adding features to analyse excel and adding the output code to the notebooks and adding analyse prepair steps to the analyse notebooks
</commit_message>
<xml_diff>
--- a/results/Comparison - LLM agent - ChatGPT - vs Graph Approach.xlsx
+++ b/results/Comparison - LLM agent - ChatGPT - vs Graph Approach.xlsx
@@ -8,15 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_Projects\_myProjects\RedundancyAndConflictAnalysis\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68D3F5EB-F9D6-45AF-87E1-4BC7697E20B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83813B85-8FD9-4B3D-9C06-51BF586A6B02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="2" xr2:uid="{54EF61F7-9983-4CF5-ABDF-2813F4BE9A2D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{54EF61F7-9983-4CF5-ABDF-2813F4BE9A2D}"/>
   </bookViews>
   <sheets>
-    <sheet name="ChatGPT-3.5-Turbo vs Graph" sheetId="1" r:id="rId1"/>
-    <sheet name="Example Comparison 3.5-turbo" sheetId="3" r:id="rId2"/>
-    <sheet name="ChatGPT-4o vs Graph" sheetId="2" r:id="rId3"/>
-    <sheet name="Example Comparison 4o" sheetId="4" r:id="rId4"/>
+    <sheet name="Graph Original Data" sheetId="5" r:id="rId1"/>
+    <sheet name="LLM 3.5 turbo output" sheetId="6" r:id="rId2"/>
+    <sheet name="LLM 4o output" sheetId="7" r:id="rId3"/>
+    <sheet name="ChatGPT-3.5-Turbo vs Graph" sheetId="1" r:id="rId4"/>
+    <sheet name="Example Comparison 3.5-turbo" sheetId="3" r:id="rId5"/>
+    <sheet name="ChatGPT-4o vs Graph" sheetId="2" r:id="rId6"/>
+    <sheet name="Example Comparison 4o" sheetId="4" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="36">
   <si>
     <t>Count of Main Part 
 Partial</t>
@@ -120,9 +123,6 @@
     <t>data set</t>
   </si>
   <si>
-    <t>LLM Agent</t>
-  </si>
-  <si>
     <t>Graph Approach</t>
   </si>
   <si>
@@ -131,12 +131,36 @@
   <si>
     <t>This data set we used for pre-training ChatGPT</t>
   </si>
+  <si>
+    <t>LLM Agent (only annotations)</t>
+  </si>
+  <si>
+    <t>LLM Agent (text + annotations)</t>
+  </si>
+  <si>
+    <t>Data set</t>
+  </si>
+  <si>
+    <t>Main Part Partial</t>
+  </si>
+  <si>
+    <t>Main Part Full</t>
+  </si>
+  <si>
+    <t>Benefit Partial</t>
+  </si>
+  <si>
+    <t>Benefit Full</t>
+  </si>
+  <si>
+    <t>From</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -167,6 +191,27 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -182,7 +227,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -223,11 +268,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -238,16 +292,38 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -581,49 +657,1237 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D20104E0-245D-46E1-AB4D-EC11DD6C59AD}">
-  <dimension ref="A1:Q22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FE89A73-71C0-4C94-B714-31DAC1CFCA7F}">
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q22" sqref="A1:Q22"/>
+      <selection activeCell="A2" sqref="A2:E22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="20">
+      <c r="A1" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+    </row>
+    <row r="2" spans="1:5" ht="42">
+      <c r="A2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="2">
+        <f>SUM(B3:B21)</f>
+        <v>0</v>
+      </c>
+      <c r="C22" s="2">
+        <f>SUM(C3:C21)</f>
+        <v>0</v>
+      </c>
+      <c r="D22" s="2">
+        <f>SUM(D3:D21)</f>
+        <v>0</v>
+      </c>
+      <c r="E22" s="2">
+        <f>SUM(E3:E21)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6862CB9B-7EBA-4643-90A5-7E237D41FFD8}">
+  <dimension ref="A1:N29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.58203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.9140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.4140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="36.58203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.9140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.4140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="20" customHeight="1">
+      <c r="A1" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="I1" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="M2" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="N2" s="13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="14"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="2"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="2"/>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="14"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="2"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="2"/>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="14"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="14"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="2"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="2"/>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="14"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="14"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="14"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="2"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="2"/>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="14"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="2"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="2"/>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="14"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="14"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="14"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="14"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" s="14"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="14"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17" s="14"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18" s="14"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" s="14"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="2"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="2"/>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20" s="14"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="2"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="2"/>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" s="14"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22" s="14"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23" s="14"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24" s="14"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="2"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="2"/>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25" s="14"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="2"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="2"/>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26" s="14"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+    </row>
+    <row r="27" spans="1:14">
+      <c r="A27" s="14"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="2"/>
+      <c r="I27" s="14"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="2"/>
+    </row>
+    <row r="28" spans="1:14">
+      <c r="A28" s="14"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="I28" s="14"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+    </row>
+    <row r="29" spans="1:14">
+      <c r="I29" s="14"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="I1:N1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE620A69-E0EE-4278-A88D-9B601C903E75}">
+  <dimension ref="A1:N29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14"/>
+  <cols>
+    <col min="1" max="1" width="36.58203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.9140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.4140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="36.58203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.9140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.4140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="20" customHeight="1">
+      <c r="A1" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="I1" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="M2" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="N2" s="15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="14"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="2"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="2"/>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="14"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="2"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="2"/>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="14"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="14"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="2"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="2"/>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="14"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="14"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="14"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="2"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="2"/>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="14"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="2"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="2"/>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="14"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="14"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="14"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="14"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" s="14"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="14"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17" s="14"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18" s="14"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" s="14"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="2"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="2"/>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20" s="14"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="2"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="2"/>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" s="14"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22" s="14"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23" s="14"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24" s="14"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="2"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="2"/>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25" s="14"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="2"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="2"/>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26" s="14"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+    </row>
+    <row r="27" spans="1:14">
+      <c r="A27" s="14"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="2"/>
+      <c r="I27" s="14"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="2"/>
+    </row>
+    <row r="28" spans="1:14">
+      <c r="A28" s="14"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="I28" s="14"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+    </row>
+    <row r="29" spans="1:14">
+      <c r="I29" s="14"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="I1:N1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D20104E0-245D-46E1-AB4D-EC11DD6C59AD}">
+  <dimension ref="A1:AJ22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14"/>
+  <cols>
+    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="8.5" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.6640625" customWidth="1"/>
-    <col min="7" max="7" width="10.25" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="32.5" customHeight="1">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:36" ht="32.5" customHeight="1">
+      <c r="A1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="T1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
+      <c r="Y1" s="6"/>
+      <c r="Z1" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="6" t="s">
+      <c r="AA1" s="8"/>
+      <c r="AB1" s="8"/>
+      <c r="AC1" s="8"/>
+      <c r="AD1" s="8"/>
+      <c r="AE1" s="6"/>
+      <c r="AF1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-    </row>
-    <row r="2" spans="1:17" ht="42">
+      <c r="AG1" s="8"/>
+      <c r="AH1" s="8"/>
+      <c r="AI1" s="8"/>
+      <c r="AJ1" s="8"/>
+    </row>
+    <row r="2" spans="1:36" ht="42">
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
@@ -669,8 +1933,53 @@
       <c r="Q2" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:17">
+      <c r="T2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:36">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -692,8 +2001,29 @@
       <c r="O3" s="2"/>
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
-    </row>
-    <row r="4" spans="1:17">
+      <c r="T3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Z3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA3" s="2"/>
+      <c r="AB3" s="2"/>
+      <c r="AC3" s="3"/>
+      <c r="AD3" s="3"/>
+      <c r="AF3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AG3" s="2"/>
+      <c r="AH3" s="2"/>
+      <c r="AI3" s="3"/>
+      <c r="AJ3" s="3"/>
+    </row>
+    <row r="4" spans="1:36">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -715,31 +2045,73 @@
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="3"/>
-    </row>
-    <row r="5" spans="1:17">
+      <c r="T4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="3"/>
+      <c r="Z4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA4" s="2"/>
+      <c r="AB4" s="2"/>
+      <c r="AC4" s="2"/>
+      <c r="AD4" s="3"/>
+      <c r="AF4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG4" s="2"/>
+      <c r="AH4" s="2"/>
+      <c r="AI4" s="2"/>
+      <c r="AJ4" s="3"/>
+    </row>
+    <row r="5" spans="1:36" ht="13.75" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="5"/>
-    </row>
-    <row r="6" spans="1:17">
+      <c r="B5" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="10"/>
+      <c r="T5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="U5" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="V5" s="4"/>
+      <c r="W5" s="4"/>
+      <c r="X5" s="4"/>
+      <c r="Y5" s="4"/>
+      <c r="Z5" s="4"/>
+      <c r="AA5" s="4"/>
+      <c r="AB5" s="4"/>
+      <c r="AC5" s="4"/>
+      <c r="AD5" s="4"/>
+      <c r="AE5" s="4"/>
+      <c r="AF5" s="4"/>
+      <c r="AG5" s="4"/>
+      <c r="AH5" s="4"/>
+      <c r="AI5" s="4"/>
+      <c r="AJ5" s="5"/>
+    </row>
+    <row r="6" spans="1:36">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -761,8 +2133,29 @@
       <c r="O6" s="2"/>
       <c r="P6" s="3"/>
       <c r="Q6" s="3"/>
-    </row>
-    <row r="7" spans="1:17">
+      <c r="T6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="U6" s="2"/>
+      <c r="V6" s="2"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="Z6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA6" s="2"/>
+      <c r="AB6" s="2"/>
+      <c r="AC6" s="3"/>
+      <c r="AD6" s="3"/>
+      <c r="AF6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="AG6" s="2"/>
+      <c r="AH6" s="2"/>
+      <c r="AI6" s="3"/>
+      <c r="AJ6" s="3"/>
+    </row>
+    <row r="7" spans="1:36">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -784,8 +2177,29 @@
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
-    </row>
-    <row r="8" spans="1:17">
+      <c r="T7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="U7" s="2"/>
+      <c r="V7" s="2"/>
+      <c r="W7" s="2"/>
+      <c r="X7" s="2"/>
+      <c r="Z7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA7" s="2"/>
+      <c r="AB7" s="2"/>
+      <c r="AC7" s="2"/>
+      <c r="AD7" s="2"/>
+      <c r="AF7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AG7" s="2"/>
+      <c r="AH7" s="2"/>
+      <c r="AI7" s="2"/>
+      <c r="AJ7" s="2"/>
+    </row>
+    <row r="8" spans="1:36">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
@@ -807,31 +2221,73 @@
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
-    </row>
-    <row r="9" spans="1:17">
+      <c r="T8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="U8" s="2"/>
+      <c r="V8" s="2"/>
+      <c r="W8" s="2"/>
+      <c r="X8" s="2"/>
+      <c r="Z8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA8" s="2"/>
+      <c r="AB8" s="2"/>
+      <c r="AC8" s="2"/>
+      <c r="AD8" s="2"/>
+      <c r="AF8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AG8" s="2"/>
+      <c r="AH8" s="2"/>
+      <c r="AI8" s="2"/>
+      <c r="AJ8" s="2"/>
+    </row>
+    <row r="9" spans="1:36" ht="13.75" customHeight="1">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
-      <c r="P9" s="4"/>
-      <c r="Q9" s="5"/>
-    </row>
-    <row r="10" spans="1:17">
+      <c r="B9" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="10"/>
+      <c r="T9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="U9" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="V9" s="4"/>
+      <c r="W9" s="4"/>
+      <c r="X9" s="4"/>
+      <c r="Y9" s="4"/>
+      <c r="Z9" s="4"/>
+      <c r="AA9" s="4"/>
+      <c r="AB9" s="4"/>
+      <c r="AC9" s="4"/>
+      <c r="AD9" s="4"/>
+      <c r="AE9" s="4"/>
+      <c r="AF9" s="4"/>
+      <c r="AG9" s="4"/>
+      <c r="AH9" s="4"/>
+      <c r="AI9" s="4"/>
+      <c r="AJ9" s="5"/>
+    </row>
+    <row r="10" spans="1:36">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
@@ -853,8 +2309,29 @@
       <c r="O10" s="2"/>
       <c r="P10" s="3"/>
       <c r="Q10" s="3"/>
-    </row>
-    <row r="11" spans="1:17">
+      <c r="T10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="U10" s="2"/>
+      <c r="V10" s="2"/>
+      <c r="W10" s="3"/>
+      <c r="X10" s="3"/>
+      <c r="Z10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA10" s="2"/>
+      <c r="AB10" s="2"/>
+      <c r="AC10" s="3"/>
+      <c r="AD10" s="3"/>
+      <c r="AF10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AG10" s="2"/>
+      <c r="AH10" s="2"/>
+      <c r="AI10" s="3"/>
+      <c r="AJ10" s="3"/>
+    </row>
+    <row r="11" spans="1:36">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -876,8 +2353,29 @@
       <c r="O11" s="2"/>
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
-    </row>
-    <row r="12" spans="1:17">
+      <c r="T11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="U11" s="2"/>
+      <c r="V11" s="2"/>
+      <c r="W11" s="2"/>
+      <c r="X11" s="2"/>
+      <c r="Z11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA11" s="2"/>
+      <c r="AB11" s="2"/>
+      <c r="AC11" s="2"/>
+      <c r="AD11" s="2"/>
+      <c r="AF11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG11" s="2"/>
+      <c r="AH11" s="2"/>
+      <c r="AI11" s="2"/>
+      <c r="AJ11" s="2"/>
+    </row>
+    <row r="12" spans="1:36">
       <c r="A12" s="2" t="s">
         <v>13</v>
       </c>
@@ -899,8 +2397,29 @@
       <c r="O12" s="2"/>
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
-    </row>
-    <row r="13" spans="1:17">
+      <c r="T12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="U12" s="2"/>
+      <c r="V12" s="2"/>
+      <c r="W12" s="2"/>
+      <c r="X12" s="2"/>
+      <c r="Z12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA12" s="2"/>
+      <c r="AB12" s="2"/>
+      <c r="AC12" s="2"/>
+      <c r="AD12" s="2"/>
+      <c r="AF12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AG12" s="2"/>
+      <c r="AH12" s="2"/>
+      <c r="AI12" s="2"/>
+      <c r="AJ12" s="2"/>
+    </row>
+    <row r="13" spans="1:36">
       <c r="A13" s="2" t="s">
         <v>14</v>
       </c>
@@ -922,8 +2441,29 @@
       <c r="O13" s="3"/>
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
-    </row>
-    <row r="14" spans="1:17">
+      <c r="T13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="U13" s="3"/>
+      <c r="V13" s="3"/>
+      <c r="W13" s="2"/>
+      <c r="X13" s="2"/>
+      <c r="Z13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA13" s="3"/>
+      <c r="AB13" s="3"/>
+      <c r="AC13" s="2"/>
+      <c r="AD13" s="2"/>
+      <c r="AF13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG13" s="3"/>
+      <c r="AH13" s="3"/>
+      <c r="AI13" s="2"/>
+      <c r="AJ13" s="2"/>
+    </row>
+    <row r="14" spans="1:36">
       <c r="A14" s="2" t="s">
         <v>15</v>
       </c>
@@ -945,8 +2485,29 @@
       <c r="O14" s="2"/>
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
-    </row>
-    <row r="15" spans="1:17">
+      <c r="T14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="U14" s="2"/>
+      <c r="V14" s="2"/>
+      <c r="W14" s="2"/>
+      <c r="X14" s="2"/>
+      <c r="Z14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA14" s="2"/>
+      <c r="AB14" s="2"/>
+      <c r="AC14" s="2"/>
+      <c r="AD14" s="2"/>
+      <c r="AF14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG14" s="2"/>
+      <c r="AH14" s="2"/>
+      <c r="AI14" s="2"/>
+      <c r="AJ14" s="2"/>
+    </row>
+    <row r="15" spans="1:36">
       <c r="A15" s="2" t="s">
         <v>16</v>
       </c>
@@ -968,8 +2529,29 @@
       <c r="O15" s="2"/>
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
-    </row>
-    <row r="16" spans="1:17">
+      <c r="T15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="U15" s="2"/>
+      <c r="V15" s="2"/>
+      <c r="W15" s="2"/>
+      <c r="X15" s="2"/>
+      <c r="Z15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA15" s="2"/>
+      <c r="AB15" s="2"/>
+      <c r="AC15" s="2"/>
+      <c r="AD15" s="2"/>
+      <c r="AF15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG15" s="2"/>
+      <c r="AH15" s="2"/>
+      <c r="AI15" s="2"/>
+      <c r="AJ15" s="2"/>
+    </row>
+    <row r="16" spans="1:36">
       <c r="A16" s="2" t="s">
         <v>17</v>
       </c>
@@ -991,8 +2573,29 @@
       <c r="O16" s="3"/>
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
-    </row>
-    <row r="17" spans="1:17">
+      <c r="T16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="U16" s="3"/>
+      <c r="V16" s="3"/>
+      <c r="W16" s="2"/>
+      <c r="X16" s="2"/>
+      <c r="Z16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA16" s="3"/>
+      <c r="AB16" s="3"/>
+      <c r="AC16" s="2"/>
+      <c r="AD16" s="2"/>
+      <c r="AF16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="AG16" s="3"/>
+      <c r="AH16" s="3"/>
+      <c r="AI16" s="2"/>
+      <c r="AJ16" s="2"/>
+    </row>
+    <row r="17" spans="1:36">
       <c r="A17" s="2" t="s">
         <v>18</v>
       </c>
@@ -1014,8 +2617,29 @@
       <c r="O17" s="2"/>
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
-    </row>
-    <row r="18" spans="1:17">
+      <c r="T17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="U17" s="2"/>
+      <c r="V17" s="2"/>
+      <c r="W17" s="2"/>
+      <c r="X17" s="2"/>
+      <c r="Z17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA17" s="2"/>
+      <c r="AB17" s="2"/>
+      <c r="AC17" s="2"/>
+      <c r="AD17" s="2"/>
+      <c r="AF17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="AG17" s="2"/>
+      <c r="AH17" s="2"/>
+      <c r="AI17" s="2"/>
+      <c r="AJ17" s="2"/>
+    </row>
+    <row r="18" spans="1:36">
       <c r="A18" s="2" t="s">
         <v>19</v>
       </c>
@@ -1037,8 +2661,29 @@
       <c r="O18" s="3"/>
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
-    </row>
-    <row r="19" spans="1:17">
+      <c r="T18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="U18" s="3"/>
+      <c r="V18" s="3"/>
+      <c r="W18" s="2"/>
+      <c r="X18" s="2"/>
+      <c r="Z18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA18" s="3"/>
+      <c r="AB18" s="3"/>
+      <c r="AC18" s="2"/>
+      <c r="AD18" s="2"/>
+      <c r="AF18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AG18" s="3"/>
+      <c r="AH18" s="3"/>
+      <c r="AI18" s="2"/>
+      <c r="AJ18" s="2"/>
+    </row>
+    <row r="19" spans="1:36">
       <c r="A19" s="2" t="s">
         <v>20</v>
       </c>
@@ -1060,8 +2705,29 @@
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
       <c r="Q19" s="3"/>
-    </row>
-    <row r="20" spans="1:17">
+      <c r="T19" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="U19" s="2"/>
+      <c r="V19" s="2"/>
+      <c r="W19" s="2"/>
+      <c r="X19" s="3"/>
+      <c r="Z19" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA19" s="2"/>
+      <c r="AB19" s="2"/>
+      <c r="AC19" s="2"/>
+      <c r="AD19" s="3"/>
+      <c r="AF19" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AG19" s="2"/>
+      <c r="AH19" s="2"/>
+      <c r="AI19" s="2"/>
+      <c r="AJ19" s="3"/>
+    </row>
+    <row r="20" spans="1:36">
       <c r="A20" s="2" t="s">
         <v>21</v>
       </c>
@@ -1083,8 +2749,29 @@
       <c r="O20" s="2"/>
       <c r="P20" s="3"/>
       <c r="Q20" s="3"/>
-    </row>
-    <row r="21" spans="1:17">
+      <c r="T20" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="U20" s="2"/>
+      <c r="V20" s="2"/>
+      <c r="W20" s="3"/>
+      <c r="X20" s="3"/>
+      <c r="Z20" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA20" s="2"/>
+      <c r="AB20" s="2"/>
+      <c r="AC20" s="3"/>
+      <c r="AD20" s="3"/>
+      <c r="AF20" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AG20" s="2"/>
+      <c r="AH20" s="2"/>
+      <c r="AI20" s="3"/>
+      <c r="AJ20" s="3"/>
+    </row>
+    <row r="21" spans="1:36">
       <c r="A21" s="2" t="s">
         <v>22</v>
       </c>
@@ -1106,8 +2793,29 @@
       <c r="O21" s="3"/>
       <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
-    </row>
-    <row r="22" spans="1:17">
+      <c r="T21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="U21" s="3"/>
+      <c r="V21" s="3"/>
+      <c r="W21" s="2"/>
+      <c r="X21" s="2"/>
+      <c r="Z21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA21" s="3"/>
+      <c r="AB21" s="3"/>
+      <c r="AC21" s="2"/>
+      <c r="AD21" s="2"/>
+      <c r="AF21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AG21" s="3"/>
+      <c r="AH21" s="3"/>
+      <c r="AI21" s="2"/>
+      <c r="AJ21" s="2"/>
+    </row>
+    <row r="22" spans="1:36">
       <c r="A22" s="2" t="s">
         <v>23</v>
       </c>
@@ -1165,20 +2873,80 @@
         <f>SUM(Q3:Q21)</f>
         <v>0</v>
       </c>
+      <c r="T22" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="U22" s="2">
+        <f>SUM(U3:U21)</f>
+        <v>0</v>
+      </c>
+      <c r="V22" s="2">
+        <f>SUM(V3:V21)</f>
+        <v>0</v>
+      </c>
+      <c r="W22" s="2">
+        <f>SUM(W3:W21)</f>
+        <v>0</v>
+      </c>
+      <c r="X22" s="2">
+        <f>SUM(X3:X21)</f>
+        <v>0</v>
+      </c>
+      <c r="Z22" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA22" s="2">
+        <f>SUM(AA3:AA21)</f>
+        <v>0</v>
+      </c>
+      <c r="AB22" s="2">
+        <f>SUM(AB3:AB21)</f>
+        <v>0</v>
+      </c>
+      <c r="AC22" s="2">
+        <f>SUM(AC3:AC21)</f>
+        <v>0</v>
+      </c>
+      <c r="AD22" s="2">
+        <f>SUM(AD3:AD21)</f>
+        <v>0</v>
+      </c>
+      <c r="AF22" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG22" s="2">
+        <f>SUM(AG3:AG21)</f>
+        <v>0</v>
+      </c>
+      <c r="AH22" s="2">
+        <f>SUM(AH3:AH21)</f>
+        <v>0</v>
+      </c>
+      <c r="AI22" s="2">
+        <f>SUM(AI3:AI21)</f>
+        <v>0</v>
+      </c>
+      <c r="AJ22" s="2">
+        <f>SUM(AJ3:AJ21)</f>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="8">
+    <mergeCell ref="B5:Q5"/>
+    <mergeCell ref="B9:Q9"/>
+    <mergeCell ref="T1:X1"/>
+    <mergeCell ref="Z1:AD1"/>
+    <mergeCell ref="AF1:AJ1"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="G1:K1"/>
     <mergeCell ref="M1:Q1"/>
-    <mergeCell ref="B5:Q5"/>
-    <mergeCell ref="B9:Q9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5F8B8F6-1E95-4BEA-B2B6-8E64712F507A}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1190,42 +2958,65 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23CBF382-5996-4BCC-89E6-F297CC73709A}">
-  <dimension ref="A1:Q22"/>
+  <dimension ref="A1:AJ22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <sheetData>
-    <row r="1" spans="1:17" ht="20">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:36" ht="20.399999999999999" customHeight="1">
+      <c r="A1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="T1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
+      <c r="Y1" s="6"/>
+      <c r="Z1" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="6" t="s">
+      <c r="AA1" s="8"/>
+      <c r="AB1" s="8"/>
+      <c r="AC1" s="8"/>
+      <c r="AD1" s="8"/>
+      <c r="AE1" s="6"/>
+      <c r="AF1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-    </row>
-    <row r="2" spans="1:17" ht="42">
+      <c r="AG1" s="8"/>
+      <c r="AH1" s="8"/>
+      <c r="AI1" s="8"/>
+      <c r="AJ1" s="8"/>
+    </row>
+    <row r="2" spans="1:36" ht="42">
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
@@ -1271,8 +3062,53 @@
       <c r="Q2" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:17">
+      <c r="T2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:36">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -1294,8 +3130,29 @@
       <c r="O3" s="2"/>
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
-    </row>
-    <row r="4" spans="1:17">
+      <c r="T3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Z3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA3" s="2"/>
+      <c r="AB3" s="2"/>
+      <c r="AC3" s="3"/>
+      <c r="AD3" s="3"/>
+      <c r="AF3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AG3" s="2"/>
+      <c r="AH3" s="2"/>
+      <c r="AI3" s="3"/>
+      <c r="AJ3" s="3"/>
+    </row>
+    <row r="4" spans="1:36">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -1317,31 +3174,73 @@
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="3"/>
-    </row>
-    <row r="5" spans="1:17">
+      <c r="T4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="3"/>
+      <c r="Z4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA4" s="2"/>
+      <c r="AB4" s="2"/>
+      <c r="AC4" s="2"/>
+      <c r="AD4" s="3"/>
+      <c r="AF4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG4" s="2"/>
+      <c r="AH4" s="2"/>
+      <c r="AI4" s="2"/>
+      <c r="AJ4" s="3"/>
+    </row>
+    <row r="5" spans="1:36" ht="13.75" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="5"/>
-    </row>
-    <row r="6" spans="1:17">
+      <c r="B5" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="10"/>
+      <c r="T5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="U5" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="V5" s="4"/>
+      <c r="W5" s="4"/>
+      <c r="X5" s="4"/>
+      <c r="Y5" s="4"/>
+      <c r="Z5" s="4"/>
+      <c r="AA5" s="4"/>
+      <c r="AB5" s="4"/>
+      <c r="AC5" s="4"/>
+      <c r="AD5" s="4"/>
+      <c r="AE5" s="4"/>
+      <c r="AF5" s="4"/>
+      <c r="AG5" s="4"/>
+      <c r="AH5" s="4"/>
+      <c r="AI5" s="4"/>
+      <c r="AJ5" s="5"/>
+    </row>
+    <row r="6" spans="1:36">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -1363,8 +3262,29 @@
       <c r="O6" s="2"/>
       <c r="P6" s="3"/>
       <c r="Q6" s="3"/>
-    </row>
-    <row r="7" spans="1:17">
+      <c r="T6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="U6" s="2"/>
+      <c r="V6" s="2"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="Z6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA6" s="2"/>
+      <c r="AB6" s="2"/>
+      <c r="AC6" s="3"/>
+      <c r="AD6" s="3"/>
+      <c r="AF6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="AG6" s="2"/>
+      <c r="AH6" s="2"/>
+      <c r="AI6" s="3"/>
+      <c r="AJ6" s="3"/>
+    </row>
+    <row r="7" spans="1:36">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -1386,8 +3306,29 @@
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
-    </row>
-    <row r="8" spans="1:17">
+      <c r="T7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="U7" s="2"/>
+      <c r="V7" s="2"/>
+      <c r="W7" s="2"/>
+      <c r="X7" s="2"/>
+      <c r="Z7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA7" s="2"/>
+      <c r="AB7" s="2"/>
+      <c r="AC7" s="2"/>
+      <c r="AD7" s="2"/>
+      <c r="AF7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AG7" s="2"/>
+      <c r="AH7" s="2"/>
+      <c r="AI7" s="2"/>
+      <c r="AJ7" s="2"/>
+    </row>
+    <row r="8" spans="1:36">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
@@ -1409,31 +3350,73 @@
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
-    </row>
-    <row r="9" spans="1:17">
+      <c r="T8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="U8" s="2"/>
+      <c r="V8" s="2"/>
+      <c r="W8" s="2"/>
+      <c r="X8" s="2"/>
+      <c r="Z8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA8" s="2"/>
+      <c r="AB8" s="2"/>
+      <c r="AC8" s="2"/>
+      <c r="AD8" s="2"/>
+      <c r="AF8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AG8" s="2"/>
+      <c r="AH8" s="2"/>
+      <c r="AI8" s="2"/>
+      <c r="AJ8" s="2"/>
+    </row>
+    <row r="9" spans="1:36" ht="13.75" customHeight="1">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
-      <c r="P9" s="4"/>
-      <c r="Q9" s="5"/>
-    </row>
-    <row r="10" spans="1:17">
+      <c r="B9" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="10"/>
+      <c r="T9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="U9" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="V9" s="4"/>
+      <c r="W9" s="4"/>
+      <c r="X9" s="4"/>
+      <c r="Y9" s="4"/>
+      <c r="Z9" s="4"/>
+      <c r="AA9" s="4"/>
+      <c r="AB9" s="4"/>
+      <c r="AC9" s="4"/>
+      <c r="AD9" s="4"/>
+      <c r="AE9" s="4"/>
+      <c r="AF9" s="4"/>
+      <c r="AG9" s="4"/>
+      <c r="AH9" s="4"/>
+      <c r="AI9" s="4"/>
+      <c r="AJ9" s="5"/>
+    </row>
+    <row r="10" spans="1:36">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
@@ -1455,8 +3438,29 @@
       <c r="O10" s="2"/>
       <c r="P10" s="3"/>
       <c r="Q10" s="3"/>
-    </row>
-    <row r="11" spans="1:17">
+      <c r="T10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="U10" s="2"/>
+      <c r="V10" s="2"/>
+      <c r="W10" s="3"/>
+      <c r="X10" s="3"/>
+      <c r="Z10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA10" s="2"/>
+      <c r="AB10" s="2"/>
+      <c r="AC10" s="3"/>
+      <c r="AD10" s="3"/>
+      <c r="AF10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AG10" s="2"/>
+      <c r="AH10" s="2"/>
+      <c r="AI10" s="3"/>
+      <c r="AJ10" s="3"/>
+    </row>
+    <row r="11" spans="1:36">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -1478,8 +3482,29 @@
       <c r="O11" s="2"/>
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
-    </row>
-    <row r="12" spans="1:17">
+      <c r="T11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="U11" s="2"/>
+      <c r="V11" s="2"/>
+      <c r="W11" s="2"/>
+      <c r="X11" s="2"/>
+      <c r="Z11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA11" s="2"/>
+      <c r="AB11" s="2"/>
+      <c r="AC11" s="2"/>
+      <c r="AD11" s="2"/>
+      <c r="AF11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG11" s="2"/>
+      <c r="AH11" s="2"/>
+      <c r="AI11" s="2"/>
+      <c r="AJ11" s="2"/>
+    </row>
+    <row r="12" spans="1:36">
       <c r="A12" s="2" t="s">
         <v>13</v>
       </c>
@@ -1501,8 +3526,29 @@
       <c r="O12" s="2"/>
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
-    </row>
-    <row r="13" spans="1:17">
+      <c r="T12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="U12" s="2"/>
+      <c r="V12" s="2"/>
+      <c r="W12" s="2"/>
+      <c r="X12" s="2"/>
+      <c r="Z12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA12" s="2"/>
+      <c r="AB12" s="2"/>
+      <c r="AC12" s="2"/>
+      <c r="AD12" s="2"/>
+      <c r="AF12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AG12" s="2"/>
+      <c r="AH12" s="2"/>
+      <c r="AI12" s="2"/>
+      <c r="AJ12" s="2"/>
+    </row>
+    <row r="13" spans="1:36">
       <c r="A13" s="2" t="s">
         <v>14</v>
       </c>
@@ -1524,8 +3570,29 @@
       <c r="O13" s="3"/>
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
-    </row>
-    <row r="14" spans="1:17">
+      <c r="T13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="U13" s="3"/>
+      <c r="V13" s="3"/>
+      <c r="W13" s="2"/>
+      <c r="X13" s="2"/>
+      <c r="Z13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA13" s="3"/>
+      <c r="AB13" s="3"/>
+      <c r="AC13" s="2"/>
+      <c r="AD13" s="2"/>
+      <c r="AF13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG13" s="3"/>
+      <c r="AH13" s="3"/>
+      <c r="AI13" s="2"/>
+      <c r="AJ13" s="2"/>
+    </row>
+    <row r="14" spans="1:36">
       <c r="A14" s="2" t="s">
         <v>15</v>
       </c>
@@ -1547,8 +3614,29 @@
       <c r="O14" s="2"/>
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
-    </row>
-    <row r="15" spans="1:17">
+      <c r="T14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="U14" s="2"/>
+      <c r="V14" s="2"/>
+      <c r="W14" s="2"/>
+      <c r="X14" s="2"/>
+      <c r="Z14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA14" s="2"/>
+      <c r="AB14" s="2"/>
+      <c r="AC14" s="2"/>
+      <c r="AD14" s="2"/>
+      <c r="AF14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG14" s="2"/>
+      <c r="AH14" s="2"/>
+      <c r="AI14" s="2"/>
+      <c r="AJ14" s="2"/>
+    </row>
+    <row r="15" spans="1:36">
       <c r="A15" s="2" t="s">
         <v>16</v>
       </c>
@@ -1570,8 +3658,29 @@
       <c r="O15" s="2"/>
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
-    </row>
-    <row r="16" spans="1:17">
+      <c r="T15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="U15" s="2"/>
+      <c r="V15" s="2"/>
+      <c r="W15" s="2"/>
+      <c r="X15" s="2"/>
+      <c r="Z15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA15" s="2"/>
+      <c r="AB15" s="2"/>
+      <c r="AC15" s="2"/>
+      <c r="AD15" s="2"/>
+      <c r="AF15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG15" s="2"/>
+      <c r="AH15" s="2"/>
+      <c r="AI15" s="2"/>
+      <c r="AJ15" s="2"/>
+    </row>
+    <row r="16" spans="1:36">
       <c r="A16" s="2" t="s">
         <v>17</v>
       </c>
@@ -1593,8 +3702,29 @@
       <c r="O16" s="3"/>
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
-    </row>
-    <row r="17" spans="1:17">
+      <c r="T16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="U16" s="3"/>
+      <c r="V16" s="3"/>
+      <c r="W16" s="2"/>
+      <c r="X16" s="2"/>
+      <c r="Z16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA16" s="3"/>
+      <c r="AB16" s="3"/>
+      <c r="AC16" s="2"/>
+      <c r="AD16" s="2"/>
+      <c r="AF16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="AG16" s="3"/>
+      <c r="AH16" s="3"/>
+      <c r="AI16" s="2"/>
+      <c r="AJ16" s="2"/>
+    </row>
+    <row r="17" spans="1:36">
       <c r="A17" s="2" t="s">
         <v>18</v>
       </c>
@@ -1616,8 +3746,29 @@
       <c r="O17" s="2"/>
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
-    </row>
-    <row r="18" spans="1:17">
+      <c r="T17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="U17" s="2"/>
+      <c r="V17" s="2"/>
+      <c r="W17" s="2"/>
+      <c r="X17" s="2"/>
+      <c r="Z17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA17" s="2"/>
+      <c r="AB17" s="2"/>
+      <c r="AC17" s="2"/>
+      <c r="AD17" s="2"/>
+      <c r="AF17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="AG17" s="2"/>
+      <c r="AH17" s="2"/>
+      <c r="AI17" s="2"/>
+      <c r="AJ17" s="2"/>
+    </row>
+    <row r="18" spans="1:36">
       <c r="A18" s="2" t="s">
         <v>19</v>
       </c>
@@ -1639,8 +3790,29 @@
       <c r="O18" s="3"/>
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
-    </row>
-    <row r="19" spans="1:17">
+      <c r="T18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="U18" s="3"/>
+      <c r="V18" s="3"/>
+      <c r="W18" s="2"/>
+      <c r="X18" s="2"/>
+      <c r="Z18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA18" s="3"/>
+      <c r="AB18" s="3"/>
+      <c r="AC18" s="2"/>
+      <c r="AD18" s="2"/>
+      <c r="AF18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AG18" s="3"/>
+      <c r="AH18" s="3"/>
+      <c r="AI18" s="2"/>
+      <c r="AJ18" s="2"/>
+    </row>
+    <row r="19" spans="1:36">
       <c r="A19" s="2" t="s">
         <v>20</v>
       </c>
@@ -1662,8 +3834,29 @@
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
       <c r="Q19" s="3"/>
-    </row>
-    <row r="20" spans="1:17">
+      <c r="T19" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="U19" s="2"/>
+      <c r="V19" s="2"/>
+      <c r="W19" s="2"/>
+      <c r="X19" s="3"/>
+      <c r="Z19" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA19" s="2"/>
+      <c r="AB19" s="2"/>
+      <c r="AC19" s="2"/>
+      <c r="AD19" s="3"/>
+      <c r="AF19" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AG19" s="2"/>
+      <c r="AH19" s="2"/>
+      <c r="AI19" s="2"/>
+      <c r="AJ19" s="3"/>
+    </row>
+    <row r="20" spans="1:36">
       <c r="A20" s="2" t="s">
         <v>21</v>
       </c>
@@ -1685,8 +3878,29 @@
       <c r="O20" s="2"/>
       <c r="P20" s="3"/>
       <c r="Q20" s="3"/>
-    </row>
-    <row r="21" spans="1:17">
+      <c r="T20" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="U20" s="2"/>
+      <c r="V20" s="2"/>
+      <c r="W20" s="3"/>
+      <c r="X20" s="3"/>
+      <c r="Z20" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA20" s="2"/>
+      <c r="AB20" s="2"/>
+      <c r="AC20" s="3"/>
+      <c r="AD20" s="3"/>
+      <c r="AF20" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AG20" s="2"/>
+      <c r="AH20" s="2"/>
+      <c r="AI20" s="3"/>
+      <c r="AJ20" s="3"/>
+    </row>
+    <row r="21" spans="1:36">
       <c r="A21" s="2" t="s">
         <v>22</v>
       </c>
@@ -1708,8 +3922,29 @@
       <c r="O21" s="3"/>
       <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
-    </row>
-    <row r="22" spans="1:17">
+      <c r="T21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="U21" s="3"/>
+      <c r="V21" s="3"/>
+      <c r="W21" s="2"/>
+      <c r="X21" s="2"/>
+      <c r="Z21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA21" s="3"/>
+      <c r="AB21" s="3"/>
+      <c r="AC21" s="2"/>
+      <c r="AD21" s="2"/>
+      <c r="AF21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AG21" s="3"/>
+      <c r="AH21" s="3"/>
+      <c r="AI21" s="2"/>
+      <c r="AJ21" s="2"/>
+    </row>
+    <row r="22" spans="1:36">
       <c r="A22" s="2" t="s">
         <v>23</v>
       </c>
@@ -1767,20 +4002,80 @@
         <f>SUM(Q3:Q21)</f>
         <v>0</v>
       </c>
+      <c r="T22" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="U22" s="2">
+        <f>SUM(U3:U21)</f>
+        <v>0</v>
+      </c>
+      <c r="V22" s="2">
+        <f>SUM(V3:V21)</f>
+        <v>0</v>
+      </c>
+      <c r="W22" s="2">
+        <f>SUM(W3:W21)</f>
+        <v>0</v>
+      </c>
+      <c r="X22" s="2">
+        <f>SUM(X3:X21)</f>
+        <v>0</v>
+      </c>
+      <c r="Z22" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA22" s="2">
+        <f>SUM(AA3:AA21)</f>
+        <v>0</v>
+      </c>
+      <c r="AB22" s="2">
+        <f>SUM(AB3:AB21)</f>
+        <v>0</v>
+      </c>
+      <c r="AC22" s="2">
+        <f>SUM(AC3:AC21)</f>
+        <v>0</v>
+      </c>
+      <c r="AD22" s="2">
+        <f>SUM(AD3:AD21)</f>
+        <v>0</v>
+      </c>
+      <c r="AF22" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG22" s="2">
+        <f>SUM(AG3:AG21)</f>
+        <v>0</v>
+      </c>
+      <c r="AH22" s="2">
+        <f>SUM(AH3:AH21)</f>
+        <v>0</v>
+      </c>
+      <c r="AI22" s="2">
+        <f>SUM(AI3:AI21)</f>
+        <v>0</v>
+      </c>
+      <c r="AJ22" s="2">
+        <f>SUM(AJ3:AJ21)</f>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="8">
+    <mergeCell ref="B5:Q5"/>
+    <mergeCell ref="B9:Q9"/>
+    <mergeCell ref="T1:X1"/>
+    <mergeCell ref="Z1:AD1"/>
+    <mergeCell ref="AF1:AJ1"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="G1:K1"/>
     <mergeCell ref="M1:Q1"/>
-    <mergeCell ref="B5:Q5"/>
-    <mergeCell ref="B9:Q9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EE9519F-93ED-4BD6-8D82-3D2D19A083F0}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Smaller improvements in notebooks and request handler
</commit_message>
<xml_diff>
--- a/results/Comparison - LLM agent - ChatGPT - vs Graph Approach.xlsx
+++ b/results/Comparison - LLM agent - ChatGPT - vs Graph Approach.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_Projects\_myProjects\RedundancyAndConflictAnalysis\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA05F78B-359E-4FD6-A96F-C98891D63867}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F27295C-6C97-465A-A3AB-DCA4A1A34355}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="5" xr2:uid="{54EF61F7-9983-4CF5-ABDF-2813F4BE9A2D}"/>
+    <workbookView xWindow="-23148" yWindow="11496" windowWidth="23256" windowHeight="13896" xr2:uid="{54EF61F7-9983-4CF5-ABDF-2813F4BE9A2D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Graph Original Data" sheetId="5" r:id="rId1"/>
-    <sheet name="LLM 3.5 turbo output" sheetId="6" r:id="rId2"/>
-    <sheet name="LLM 4o output" sheetId="7" r:id="rId3"/>
-    <sheet name="ChatGPT-3.5-Turbo vs Graph" sheetId="1" r:id="rId4"/>
-    <sheet name="Example Comparison 3.5-turbo" sheetId="3" r:id="rId5"/>
-    <sheet name="ChatGPT-4o vs Graph" sheetId="2" r:id="rId6"/>
-    <sheet name="Example Comparison 4o" sheetId="4" r:id="rId7"/>
+    <sheet name="Graph Redundancy Data" sheetId="8" r:id="rId1"/>
+    <sheet name="Graph Original Data" sheetId="5" r:id="rId2"/>
+    <sheet name="LLM 3.5 turbo output" sheetId="6" r:id="rId3"/>
+    <sheet name="LLM 4o output" sheetId="7" r:id="rId4"/>
+    <sheet name="ChatGPT-3.5-Turbo vs Graph" sheetId="1" r:id="rId5"/>
+    <sheet name="Example Comparison 3.5-turbo" sheetId="3" r:id="rId6"/>
+    <sheet name="ChatGPT-4o vs Graph" sheetId="2" r:id="rId7"/>
+    <sheet name="Example Comparison 4o" sheetId="4" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="48">
   <si>
     <t>Count of Main Part 
 Partial</t>
@@ -154,6 +155,48 @@
   </si>
   <si>
     <t>From</t>
+  </si>
+  <si>
+    <t>* Number of total redundancy clauses between the pairs containing trigger edges (if there is no redundancy clause in the main part of the sentence, the redundancies in persona are not counted)
+** Number of Redundancy clauses in the main part of the sentence that also contain triggers if there is a Redundancy between primary action and primary entity
+*** Number of Redundancy clauses in the benefit part of the sentence (without counting the persona)</t>
+  </si>
+  <si>
+    <t>Items</t>
+  </si>
+  <si>
+    <t>Project Number</t>
+  </si>
+  <si>
+    <t>Redundant Pairs</t>
+  </si>
+  <si>
+    <t>User Stories Texts</t>
+  </si>
+  <si>
+    <t>Total Redundancy Clause *</t>
+  </si>
+  <si>
+    <t>Main Part Redundancy Clause**</t>
+  </si>
+  <si>
+    <t>Benefit Part Redundancy Clause ***</t>
+  </si>
+  <si>
+    <t>Main Part 
+Partial</t>
+  </si>
+  <si>
+    <t>Main Part 
+Full</t>
+  </si>
+  <si>
+    <t>Benefit
+Partial</t>
+  </si>
+  <si>
+    <t>Benefit
+Full</t>
   </si>
 </sst>
 </file>
@@ -281,7 +324,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -322,6 +365,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -657,6 +712,78 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC821718-B532-45EA-A1D5-6CFE5A4C259A}">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetData>
+    <row r="1" spans="1:13" ht="93.5" customHeight="1">
+      <c r="A1" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+    </row>
+    <row r="2" spans="1:13" ht="67">
+      <c r="A2" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="J2" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="L2" s="17"/>
+      <c r="M2" s="18"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:K1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FE89A73-71C0-4C94-B714-31DAC1CFCA7F}">
   <dimension ref="A1:E22"/>
   <sheetViews>
@@ -1044,7 +1171,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6862CB9B-7EBA-4643-90A5-7E237D41FFD8}">
   <dimension ref="A1:N29"/>
   <sheetViews>
@@ -1507,7 +1634,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE620A69-E0EE-4278-A88D-9B601C903E75}">
   <dimension ref="A1:N29"/>
   <sheetViews>
@@ -1970,7 +2097,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D20104E0-245D-46E1-AB4D-EC11DD6C59AD}">
   <dimension ref="A1:AJ22"/>
   <sheetViews>
@@ -2039,7 +2166,7 @@
       <c r="AI1" s="12"/>
       <c r="AJ1" s="12"/>
     </row>
-    <row r="2" spans="1:36" ht="42">
+    <row r="2" spans="1:36" ht="56">
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
@@ -3098,7 +3225,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5F8B8F6-1E95-4BEA-B2B6-8E64712F507A}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -3110,11 +3237,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23CBF382-5996-4BCC-89E6-F297CC73709A}">
   <dimension ref="A1:AJ22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
@@ -3168,7 +3295,7 @@
       <c r="AI1" s="12"/>
       <c r="AJ1" s="12"/>
     </row>
-    <row r="2" spans="1:36" ht="42">
+    <row r="2" spans="1:36" ht="56">
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
@@ -4227,7 +4354,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EE9519F-93ED-4BD6-8D82-3D2D19A083F0}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>